<commit_message>
Stop tracking .venv and update .gitignore
</commit_message>
<xml_diff>
--- a/1.2.1 assessment_data.xlsx
+++ b/1.2.1 assessment_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC152"/>
+  <dimension ref="A1:AC164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16121,6 +16121,1294 @@
         <v>0</v>
       </c>
     </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>ਅਮੁਲ ਗੁਣ ਅਮੁਲ ਵਾਪਾਰ ॥</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Priceless qualities, priceless transactions.</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>ਅਮੁਲ</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>ਅਮੋਲਕ</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>ਅਮੁਲ</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>Plural / ਬਹੁ</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>Qualitative ਗੁਣ</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>Adjectives / ਵਿਸ਼ੇਸ਼ਣ</t>
+        </is>
+      </c>
+      <c r="L153" t="n">
+        <v>1</v>
+      </c>
+      <c r="M153" t="n">
+        <v>0</v>
+      </c>
+      <c r="N153" t="n">
+        <v>240</v>
+      </c>
+      <c r="O153" t="n">
+        <v>240</v>
+      </c>
+      <c r="P153" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q153" t="n">
+        <v>1</v>
+      </c>
+      <c r="R153" t="inlineStr"/>
+      <c r="S153" t="inlineStr"/>
+      <c r="T153" t="inlineStr">
+        <is>
+          <t>ਮਹਲਾ ੧</t>
+        </is>
+      </c>
+      <c r="U153" t="inlineStr"/>
+      <c r="V153" t="inlineStr"/>
+      <c r="W153" t="inlineStr">
+        <is>
+          <t>ਜਪੁ</t>
+        </is>
+      </c>
+      <c r="X153" t="inlineStr"/>
+      <c r="Y153" t="inlineStr">
+        <is>
+          <t>ਸ਼ਬਦ</t>
+        </is>
+      </c>
+      <c r="Z153" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA153" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC153" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>ਅਮੁਲ ਗੁਣ ਅਮੁਲ ਵਾਪਾਰ ॥</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Priceless qualities, priceless transactions.</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr"/>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>ਗੁਣ</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>ਸ਼ਿਵ ਜੀ ਦੇ ਸੇਵਕ| ਗੁਣਾਂ ਦੇ ਕਾਰਨ| ਖ਼ੋਆਂ</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>Plural / ਬਹੁ</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>Nominative ਕਰਤਾ</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L154" t="n">
+        <v>1</v>
+      </c>
+      <c r="M154" t="n">
+        <v>1</v>
+      </c>
+      <c r="N154" t="n">
+        <v>240</v>
+      </c>
+      <c r="O154" t="n">
+        <v>240</v>
+      </c>
+      <c r="P154" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q154" t="n">
+        <v>1</v>
+      </c>
+      <c r="R154" t="inlineStr"/>
+      <c r="S154" t="inlineStr"/>
+      <c r="T154" t="inlineStr">
+        <is>
+          <t>ਮਹਲਾ ੧</t>
+        </is>
+      </c>
+      <c r="U154" t="inlineStr"/>
+      <c r="V154" t="inlineStr"/>
+      <c r="W154" t="inlineStr">
+        <is>
+          <t>ਜਪੁ</t>
+        </is>
+      </c>
+      <c r="X154" t="inlineStr"/>
+      <c r="Y154" t="inlineStr">
+        <is>
+          <t>ਸ਼ਬਦ</t>
+        </is>
+      </c>
+      <c r="Z154" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA154" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC154" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>ਅਮੁਲ ਗੁਣ ਅਮੁਲ ਵਾਪਾਰ ॥</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Priceless qualities, priceless transactions.</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr"/>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>ਅਮੁਲ</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>ਅਮੋਲਕ</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>ਅਮੁਲ</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>Plural / ਬਹੁ</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>Qualitative ਗੁਣ</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>Adjectives / ਵਿਸ਼ੇਸ਼ਣ</t>
+        </is>
+      </c>
+      <c r="L155" t="n">
+        <v>1</v>
+      </c>
+      <c r="M155" t="n">
+        <v>2</v>
+      </c>
+      <c r="N155" t="n">
+        <v>240</v>
+      </c>
+      <c r="O155" t="n">
+        <v>240</v>
+      </c>
+      <c r="P155" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q155" t="n">
+        <v>1</v>
+      </c>
+      <c r="R155" t="inlineStr"/>
+      <c r="S155" t="inlineStr"/>
+      <c r="T155" t="inlineStr">
+        <is>
+          <t>ਮਹਲਾ ੧</t>
+        </is>
+      </c>
+      <c r="U155" t="inlineStr"/>
+      <c r="V155" t="inlineStr"/>
+      <c r="W155" t="inlineStr">
+        <is>
+          <t>ਜਪੁ</t>
+        </is>
+      </c>
+      <c r="X155" t="inlineStr"/>
+      <c r="Y155" t="inlineStr">
+        <is>
+          <t>ਸ਼ਬਦ</t>
+        </is>
+      </c>
+      <c r="Z155" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA155" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB155" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC155" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>ਮੇਰਾ ਪ੍ਰਭੁ ਹੈ ਗੁਣ ਕਾ ਦਾਤਾ ਅਵਗਣ ਸਬਦਿ ਜਲਾਏ ॥</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>My Lord is the giver of virtues; vices He burns through the Word.</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr"/>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>ਮੇਰਾ</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>ਮੇਰਾ</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>ਮੇਰਾ</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>Possessive Pronominal / ਸੰਬੰਧ ਦਰਸਾਊ</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>1st Person / ਉੱਤਮ ਪੁਰਖ</t>
+        </is>
+      </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>Adjectives / ਵਿਸ਼ੇਸ਼ਣ</t>
+        </is>
+      </c>
+      <c r="L156" t="n">
+        <v>1</v>
+      </c>
+      <c r="M156" t="n">
+        <v>0</v>
+      </c>
+      <c r="N156" t="n">
+        <v>45230</v>
+      </c>
+      <c r="O156" t="n">
+        <v>7</v>
+      </c>
+      <c r="P156" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q156" t="n">
+        <v>2836</v>
+      </c>
+      <c r="R156" t="inlineStr">
+        <is>
+          <t>ਭੈਰਉ</t>
+        </is>
+      </c>
+      <c r="S156" t="inlineStr"/>
+      <c r="T156" t="inlineStr">
+        <is>
+          <t>ਮਹਲਾ ੩</t>
+        </is>
+      </c>
+      <c r="U156" t="inlineStr"/>
+      <c r="V156" t="inlineStr"/>
+      <c r="W156" t="inlineStr"/>
+      <c r="X156" t="inlineStr">
+        <is>
+          <t>ਘਰੁ ੨</t>
+        </is>
+      </c>
+      <c r="Y156" t="inlineStr">
+        <is>
+          <t>ਸ਼ਬਦ</t>
+        </is>
+      </c>
+      <c r="Z156" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA156" t="n">
+        <v>1131</v>
+      </c>
+      <c r="AB156" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC156" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>ਮੇਰਾ ਪ੍ਰਭੁ ਹੈ ਗੁਣ ਕਾ ਦਾਤਾ ਅਵਗਣ ਸਬਦਿ ਜਲਾਏ ॥</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>My Lord is the giver of virtues; vices He burns through the Word.</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr"/>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>ਪ੍ਰਭੁ</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>ਮਾਲਕ</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>ੁ</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>Nominative ਕਰਤਾ</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L157" t="n">
+        <v>1</v>
+      </c>
+      <c r="M157" t="n">
+        <v>1</v>
+      </c>
+      <c r="N157" t="n">
+        <v>45230</v>
+      </c>
+      <c r="O157" t="n">
+        <v>7</v>
+      </c>
+      <c r="P157" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q157" t="n">
+        <v>2836</v>
+      </c>
+      <c r="R157" t="inlineStr">
+        <is>
+          <t>ਭੈਰਉ</t>
+        </is>
+      </c>
+      <c r="S157" t="inlineStr"/>
+      <c r="T157" t="inlineStr">
+        <is>
+          <t>ਮਹਲਾ ੩</t>
+        </is>
+      </c>
+      <c r="U157" t="inlineStr"/>
+      <c r="V157" t="inlineStr"/>
+      <c r="W157" t="inlineStr"/>
+      <c r="X157" t="inlineStr">
+        <is>
+          <t>ਘਰੁ ੨</t>
+        </is>
+      </c>
+      <c r="Y157" t="inlineStr">
+        <is>
+          <t>ਸ਼ਬਦ</t>
+        </is>
+      </c>
+      <c r="Z157" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA157" t="n">
+        <v>1131</v>
+      </c>
+      <c r="AB157" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC157" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>ਮੇਰਾ ਪ੍ਰਭੁ ਹੈ ਗੁਣ ਕਾ ਦਾਤਾ ਅਵਗਣ ਸਬਦਿ ਜਲਾਏ ॥</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>My Lord is the giver of virtues; vices He burns through the Word.</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr"/>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>ਹੈ</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>ਹੈਂ</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>ਹੈ</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>Auxiliary ਅਪੁਰਨ Present</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>Trans / ਨਪੁਂਸਕ</t>
+        </is>
+      </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>3rd Person / ਅਨਯ ਪੁਰਖ</t>
+        </is>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>Verb / ਕਿਰਿਆ</t>
+        </is>
+      </c>
+      <c r="L158" t="n">
+        <v>1</v>
+      </c>
+      <c r="M158" t="n">
+        <v>2</v>
+      </c>
+      <c r="N158" t="n">
+        <v>45230</v>
+      </c>
+      <c r="O158" t="n">
+        <v>7</v>
+      </c>
+      <c r="P158" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q158" t="n">
+        <v>2836</v>
+      </c>
+      <c r="R158" t="inlineStr">
+        <is>
+          <t>ਭੈਰਉ</t>
+        </is>
+      </c>
+      <c r="S158" t="inlineStr"/>
+      <c r="T158" t="inlineStr">
+        <is>
+          <t>ਮਹਲਾ ੩</t>
+        </is>
+      </c>
+      <c r="U158" t="inlineStr"/>
+      <c r="V158" t="inlineStr"/>
+      <c r="W158" t="inlineStr"/>
+      <c r="X158" t="inlineStr">
+        <is>
+          <t>ਘਰੁ ੨</t>
+        </is>
+      </c>
+      <c r="Y158" t="inlineStr">
+        <is>
+          <t>ਸ਼ਬਦ</t>
+        </is>
+      </c>
+      <c r="Z158" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA158" t="n">
+        <v>1131</v>
+      </c>
+      <c r="AB158" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC158" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>ਮੇਰਾ ਪ੍ਰਭੁ ਹੈ ਗੁਣ ਕਾ ਦਾਤਾ ਅਵਗਣ ਸਬਦਿ ਜਲਾਏ ॥</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>My Lord is the giver of virtues; vices He burns through the Word.</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr"/>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>ਗੁਣ</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>ਸਰਗੁਣ</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>Plural / ਬਹੁ</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>Dative ਸੰਪ੍ਦਾਨ</t>
+        </is>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L159" t="n">
+        <v>1</v>
+      </c>
+      <c r="M159" t="n">
+        <v>3</v>
+      </c>
+      <c r="N159" t="n">
+        <v>45230</v>
+      </c>
+      <c r="O159" t="n">
+        <v>7</v>
+      </c>
+      <c r="P159" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q159" t="n">
+        <v>2836</v>
+      </c>
+      <c r="R159" t="inlineStr">
+        <is>
+          <t>ਭੈਰਉ</t>
+        </is>
+      </c>
+      <c r="S159" t="inlineStr"/>
+      <c r="T159" t="inlineStr">
+        <is>
+          <t>ਮਹਲਾ ੩</t>
+        </is>
+      </c>
+      <c r="U159" t="inlineStr"/>
+      <c r="V159" t="inlineStr"/>
+      <c r="W159" t="inlineStr"/>
+      <c r="X159" t="inlineStr">
+        <is>
+          <t>ਘਰੁ ੨</t>
+        </is>
+      </c>
+      <c r="Y159" t="inlineStr">
+        <is>
+          <t>ਸ਼ਬਦ</t>
+        </is>
+      </c>
+      <c r="Z159" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA159" t="n">
+        <v>1131</v>
+      </c>
+      <c r="AB159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC159" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>ਮੇਰਾ ਪ੍ਰਭੁ ਹੈ ਗੁਣ ਕਾ ਦਾਤਾ ਅਵਗਣ ਸਬਦਿ ਜਲਾਏ ॥</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>My Lord is the giver of virtues; vices He burns through the Word.</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr"/>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>ਕਾ</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>ਦਾ</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>ਕਾ</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>Of</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J160" t="inlineStr"/>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>Postposition / ਸੰਬੰਧਕ</t>
+        </is>
+      </c>
+      <c r="L160" t="n">
+        <v>1</v>
+      </c>
+      <c r="M160" t="n">
+        <v>4</v>
+      </c>
+      <c r="N160" t="n">
+        <v>45230</v>
+      </c>
+      <c r="O160" t="n">
+        <v>7</v>
+      </c>
+      <c r="P160" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q160" t="n">
+        <v>2836</v>
+      </c>
+      <c r="R160" t="inlineStr">
+        <is>
+          <t>ਭੈਰਉ</t>
+        </is>
+      </c>
+      <c r="S160" t="inlineStr"/>
+      <c r="T160" t="inlineStr">
+        <is>
+          <t>ਮਹਲਾ ੩</t>
+        </is>
+      </c>
+      <c r="U160" t="inlineStr"/>
+      <c r="V160" t="inlineStr"/>
+      <c r="W160" t="inlineStr"/>
+      <c r="X160" t="inlineStr">
+        <is>
+          <t>ਘਰੁ ੨</t>
+        </is>
+      </c>
+      <c r="Y160" t="inlineStr">
+        <is>
+          <t>ਸ਼ਬਦ</t>
+        </is>
+      </c>
+      <c r="Z160" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA160" t="n">
+        <v>1131</v>
+      </c>
+      <c r="AB160" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC160" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>ਮੇਰਾ ਪ੍ਰਭੁ ਹੈ ਗੁਣ ਕਾ ਦਾਤਾ ਅਵਗਣ ਸਬਦਿ ਜਲਾਏ ॥</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>My Lord is the giver of virtues; vices He burns through the Word.</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr"/>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>ਦਾਤਾ</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>ਦੇਣ ਵਾਲਾ</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>ਕਰਤਾ</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>Nominative ਕਰਤਾ</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>ਕਨਾੱ Ending</t>
+        </is>
+      </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L161" t="n">
+        <v>1</v>
+      </c>
+      <c r="M161" t="n">
+        <v>5</v>
+      </c>
+      <c r="N161" t="n">
+        <v>45230</v>
+      </c>
+      <c r="O161" t="n">
+        <v>7</v>
+      </c>
+      <c r="P161" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q161" t="n">
+        <v>2836</v>
+      </c>
+      <c r="R161" t="inlineStr">
+        <is>
+          <t>ਭੈਰਉ</t>
+        </is>
+      </c>
+      <c r="S161" t="inlineStr"/>
+      <c r="T161" t="inlineStr">
+        <is>
+          <t>ਮਹਲਾ ੩</t>
+        </is>
+      </c>
+      <c r="U161" t="inlineStr"/>
+      <c r="V161" t="inlineStr"/>
+      <c r="W161" t="inlineStr"/>
+      <c r="X161" t="inlineStr">
+        <is>
+          <t>ਘਰੁ ੨</t>
+        </is>
+      </c>
+      <c r="Y161" t="inlineStr">
+        <is>
+          <t>ਸ਼ਬਦ</t>
+        </is>
+      </c>
+      <c r="Z161" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA161" t="n">
+        <v>1131</v>
+      </c>
+      <c r="AB161" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC161" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>ਮੇਰਾ ਪ੍ਰਭੁ ਹੈ ਗੁਣ ਕਾ ਦਾਤਾ ਅਵਗਣ ਸਬਦਿ ਜਲਾਏ ॥</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>My Lord is the giver of virtues; vices He burns through the Word.</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr"/>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>ਅਵਗਣ</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr"/>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>Plural / ਬਹੁ</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>Accusative ਕਰਮ</t>
+        </is>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L162" t="n">
+        <v>1</v>
+      </c>
+      <c r="M162" t="n">
+        <v>6</v>
+      </c>
+      <c r="N162" t="n">
+        <v>45230</v>
+      </c>
+      <c r="O162" t="n">
+        <v>7</v>
+      </c>
+      <c r="P162" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q162" t="n">
+        <v>2836</v>
+      </c>
+      <c r="R162" t="inlineStr">
+        <is>
+          <t>ਭੈਰਉ</t>
+        </is>
+      </c>
+      <c r="S162" t="inlineStr"/>
+      <c r="T162" t="inlineStr">
+        <is>
+          <t>ਮਹਲਾ ੩</t>
+        </is>
+      </c>
+      <c r="U162" t="inlineStr"/>
+      <c r="V162" t="inlineStr"/>
+      <c r="W162" t="inlineStr"/>
+      <c r="X162" t="inlineStr">
+        <is>
+          <t>ਘਰੁ ੨</t>
+        </is>
+      </c>
+      <c r="Y162" t="inlineStr">
+        <is>
+          <t>ਸ਼ਬਦ</t>
+        </is>
+      </c>
+      <c r="Z162" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA162" t="n">
+        <v>1131</v>
+      </c>
+      <c r="AB162" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC162" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>ਮੇਰਾ ਪ੍ਰਭੁ ਹੈ ਗੁਣ ਕਾ ਦਾਤਾ ਅਵਗਣ ਸਬਦਿ ਜਲਾਏ ॥</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>My Lord is the giver of virtues; vices He burns through the Word.</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr"/>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>ਸਬਦਿ</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>ਆਪਣੇ ਸ਼ਬਦ ਦੀ ਰਾਹੀਂ| ਸ਼ਬਦ ਦੁਆਰਾ| ਸ਼ਬਦ ਨਾਲ</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>ਸਬਦਿ</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>Instrumental ਕਰਣ</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L163" t="n">
+        <v>1</v>
+      </c>
+      <c r="M163" t="n">
+        <v>7</v>
+      </c>
+      <c r="N163" t="n">
+        <v>45230</v>
+      </c>
+      <c r="O163" t="n">
+        <v>7</v>
+      </c>
+      <c r="P163" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q163" t="n">
+        <v>2836</v>
+      </c>
+      <c r="R163" t="inlineStr">
+        <is>
+          <t>ਭੈਰਉ</t>
+        </is>
+      </c>
+      <c r="S163" t="inlineStr"/>
+      <c r="T163" t="inlineStr">
+        <is>
+          <t>ਮਹਲਾ ੩</t>
+        </is>
+      </c>
+      <c r="U163" t="inlineStr"/>
+      <c r="V163" t="inlineStr"/>
+      <c r="W163" t="inlineStr"/>
+      <c r="X163" t="inlineStr">
+        <is>
+          <t>ਘਰੁ ੨</t>
+        </is>
+      </c>
+      <c r="Y163" t="inlineStr">
+        <is>
+          <t>ਸ਼ਬਦ</t>
+        </is>
+      </c>
+      <c r="Z163" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA163" t="n">
+        <v>1131</v>
+      </c>
+      <c r="AB163" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC163" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>ਮੇਰਾ ਪ੍ਰਭੁ ਹੈ ਗੁਣ ਕਾ ਦਾਤਾ ਅਵਗਣ ਸਬਦਿ ਜਲਾਏ ॥</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>My Lord is the giver of virtues; vices He burns through the Word.</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr"/>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>ਜਲਾਏ</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>ਸਾੜਦਾ ਹੈ</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>ਆਖਾਏ</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>Causative ਪੇ੍ਰਣਾਰਥਕ</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>Trans / ਨਪੁਂਸਕ</t>
+        </is>
+      </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>3rd Person / ਅਨਯ ਪੁਰਖ</t>
+        </is>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>Verb / ਕਿਰਿਆ</t>
+        </is>
+      </c>
+      <c r="L164" t="n">
+        <v>1</v>
+      </c>
+      <c r="M164" t="n">
+        <v>8</v>
+      </c>
+      <c r="N164" t="n">
+        <v>45230</v>
+      </c>
+      <c r="O164" t="n">
+        <v>7</v>
+      </c>
+      <c r="P164" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q164" t="n">
+        <v>2836</v>
+      </c>
+      <c r="R164" t="inlineStr">
+        <is>
+          <t>ਭੈਰਉ</t>
+        </is>
+      </c>
+      <c r="S164" t="inlineStr"/>
+      <c r="T164" t="inlineStr">
+        <is>
+          <t>ਮਹਲਾ ੩</t>
+        </is>
+      </c>
+      <c r="U164" t="inlineStr"/>
+      <c r="V164" t="inlineStr"/>
+      <c r="W164" t="inlineStr"/>
+      <c r="X164" t="inlineStr">
+        <is>
+          <t>ਘਰੁ ੨</t>
+        </is>
+      </c>
+      <c r="Y164" t="inlineStr">
+        <is>
+          <t>ਸ਼ਬਦ</t>
+        </is>
+      </c>
+      <c r="Z164" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA164" t="n">
+        <v>1131</v>
+      </c>
+      <c r="AB164" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC164" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the specified endings list to include "ਏ"
</commit_message>
<xml_diff>
--- a/1.2.1 assessment_data.xlsx
+++ b/1.2.1 assessment_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC231"/>
+  <dimension ref="A1:AC240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24226,6 +24226,935 @@
         <v>0</v>
       </c>
     </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਮਨੁ ਜਾਨੈ ਸਭ ਬਾਤ ਜਾਨਤ ਹੀ ਅਉਗਨੁ ਕਰੈ ॥</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr"/>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>ਹੇ ਕਬੀਰ!</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ</t>
+        </is>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>Vocative ਸੰਬੋਧਨ</t>
+        </is>
+      </c>
+      <c r="I232" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J232" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K232" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L232" t="n">
+        <v>1</v>
+      </c>
+      <c r="M232" t="n">
+        <v>0</v>
+      </c>
+      <c r="N232" t="n">
+        <v>54730</v>
+      </c>
+      <c r="O232" t="n">
+        <v>1</v>
+      </c>
+      <c r="P232" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q232" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S232" t="inlineStr"/>
+      <c r="T232" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U232" t="inlineStr"/>
+      <c r="V232" t="inlineStr"/>
+      <c r="W232" t="inlineStr"/>
+      <c r="X232" t="inlineStr"/>
+      <c r="Y232" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z232" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA232" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB232" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC232" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਮਨੁ ਜਾਨੈ ਸਭ ਬਾਤ ਜਾਨਤ ਹੀ ਅਉਗਨੁ ਕਰੈ ॥</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr"/>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>ਮਨੁ</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>ਮਨ</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>ਮਨੁ</t>
+        </is>
+      </c>
+      <c r="G233" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>Nominative ਕਰਤਾ</t>
+        </is>
+      </c>
+      <c r="I233" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J233" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K233" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L233" t="n">
+        <v>1</v>
+      </c>
+      <c r="M233" t="n">
+        <v>1</v>
+      </c>
+      <c r="N233" t="n">
+        <v>54730</v>
+      </c>
+      <c r="O233" t="n">
+        <v>1</v>
+      </c>
+      <c r="P233" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q233" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R233" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S233" t="inlineStr"/>
+      <c r="T233" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U233" t="inlineStr"/>
+      <c r="V233" t="inlineStr"/>
+      <c r="W233" t="inlineStr"/>
+      <c r="X233" t="inlineStr"/>
+      <c r="Y233" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z233" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA233" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB233" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC233" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਮਨੁ ਜਾਨੈ ਸਭ ਬਾਤ ਜਾਨਤ ਹੀ ਅਉਗਨੁ ਕਰੈ ॥</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr"/>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>ਜਾਨੈ</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>ਜਾਣਦਾ ਹੈ| ਸਮਝਦਾ ਹੈ| ਪਛਾਣਦਾ ਹੈ</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>ੈ</t>
+        </is>
+      </c>
+      <c r="G234" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>Present ਵਰਤਮਾਨ</t>
+        </is>
+      </c>
+      <c r="I234" t="inlineStr">
+        <is>
+          <t>Trans / ਨਪੁਂਸਕ</t>
+        </is>
+      </c>
+      <c r="J234" t="inlineStr">
+        <is>
+          <t>3rd Person / ਅਨਯ ਪੁਰਖ</t>
+        </is>
+      </c>
+      <c r="K234" t="inlineStr">
+        <is>
+          <t>Verb / ਕਿਰਿਆ</t>
+        </is>
+      </c>
+      <c r="L234" t="n">
+        <v>1</v>
+      </c>
+      <c r="M234" t="n">
+        <v>2</v>
+      </c>
+      <c r="N234" t="n">
+        <v>54730</v>
+      </c>
+      <c r="O234" t="n">
+        <v>1</v>
+      </c>
+      <c r="P234" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q234" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S234" t="inlineStr"/>
+      <c r="T234" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U234" t="inlineStr"/>
+      <c r="V234" t="inlineStr"/>
+      <c r="W234" t="inlineStr"/>
+      <c r="X234" t="inlineStr"/>
+      <c r="Y234" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z234" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA234" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB234" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC234" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਮਨੁ ਜਾਨੈ ਸਭ ਬਾਤ ਜਾਨਤ ਹੀ ਅਉਗਨੁ ਕਰੈ ॥</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr"/>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>ਸਭ</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>ਹਰੇਕ| ਸਾਰੀ</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>ਸਭ</t>
+        </is>
+      </c>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>Indefinite / ਅਨਿਸਚੇ ਵਾਚਕ</t>
+        </is>
+      </c>
+      <c r="I235" t="inlineStr">
+        <is>
+          <t>Feminine / ਇਸਤਰੀ</t>
+        </is>
+      </c>
+      <c r="J235" t="inlineStr"/>
+      <c r="K235" t="inlineStr">
+        <is>
+          <t>Adjectives / ਵਿਸ਼ੇਸ਼ਣ</t>
+        </is>
+      </c>
+      <c r="L235" t="n">
+        <v>1</v>
+      </c>
+      <c r="M235" t="n">
+        <v>3</v>
+      </c>
+      <c r="N235" t="n">
+        <v>54730</v>
+      </c>
+      <c r="O235" t="n">
+        <v>1</v>
+      </c>
+      <c r="P235" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q235" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S235" t="inlineStr"/>
+      <c r="T235" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U235" t="inlineStr"/>
+      <c r="V235" t="inlineStr"/>
+      <c r="W235" t="inlineStr"/>
+      <c r="X235" t="inlineStr"/>
+      <c r="Y235" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z235" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA235" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB235" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC235" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਮਨੁ ਜਾਨੈ ਸਭ ਬਾਤ ਜਾਨਤ ਹੀ ਅਉਗਨੁ ਕਰੈ ॥</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr"/>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>ਬਾਤ</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>ਗੱਲ| ਕਹਾਣੀ</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ</t>
+        </is>
+      </c>
+      <c r="G236" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>Accusative ਕਰਮ</t>
+        </is>
+      </c>
+      <c r="I236" t="inlineStr">
+        <is>
+          <t>Feminine / ਇਸਤਰੀ</t>
+        </is>
+      </c>
+      <c r="J236" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K236" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L236" t="n">
+        <v>1</v>
+      </c>
+      <c r="M236" t="n">
+        <v>4</v>
+      </c>
+      <c r="N236" t="n">
+        <v>54730</v>
+      </c>
+      <c r="O236" t="n">
+        <v>1</v>
+      </c>
+      <c r="P236" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q236" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S236" t="inlineStr"/>
+      <c r="T236" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U236" t="inlineStr"/>
+      <c r="V236" t="inlineStr"/>
+      <c r="W236" t="inlineStr"/>
+      <c r="X236" t="inlineStr"/>
+      <c r="Y236" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z236" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA236" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB236" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC236" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਮਨੁ ਜਾਨੈ ਸਭ ਬਾਤ ਜਾਨਤ ਹੀ ਅਉਗਨੁ ਕਰੈ ॥</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr"/>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>ਜਾਨਤ</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>ਜਾਣਦਾ ਹੋਇਆ</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>ਕਰਤ</t>
+        </is>
+      </c>
+      <c r="G237" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H237" t="inlineStr">
+        <is>
+          <t>Present ਵਰਤਮਾਨ (Participle form)</t>
+        </is>
+      </c>
+      <c r="I237" t="inlineStr">
+        <is>
+          <t>Trans / ਨਪੁਂਸਕ</t>
+        </is>
+      </c>
+      <c r="J237" t="inlineStr">
+        <is>
+          <t>3rd Person / ਅਨਯ ਪੁਰਖ</t>
+        </is>
+      </c>
+      <c r="K237" t="inlineStr">
+        <is>
+          <t>Verb / ਕਿਰਿਆ</t>
+        </is>
+      </c>
+      <c r="L237" t="n">
+        <v>1</v>
+      </c>
+      <c r="M237" t="n">
+        <v>5</v>
+      </c>
+      <c r="N237" t="n">
+        <v>54730</v>
+      </c>
+      <c r="O237" t="n">
+        <v>1</v>
+      </c>
+      <c r="P237" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q237" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S237" t="inlineStr"/>
+      <c r="T237" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U237" t="inlineStr"/>
+      <c r="V237" t="inlineStr"/>
+      <c r="W237" t="inlineStr"/>
+      <c r="X237" t="inlineStr"/>
+      <c r="Y237" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z237" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA237" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB237" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC237" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਮਨੁ ਜਾਨੈ ਸਭ ਬਾਤ ਜਾਨਤ ਹੀ ਅਉਗਨੁ ਕਰੈ ॥</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr"/>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>ਹੀ</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>ਹੀ</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>ਹੀ</t>
+        </is>
+      </c>
+      <c r="G238" t="inlineStr"/>
+      <c r="H238" t="inlineStr">
+        <is>
+          <t>Sress / Emphasis / ਤਾਕੀਦ ਵਾਚਕ</t>
+        </is>
+      </c>
+      <c r="I238" t="inlineStr"/>
+      <c r="J238" t="inlineStr"/>
+      <c r="K238" t="inlineStr">
+        <is>
+          <t>Adverb / ਕਿਰਿਆ ਵਿਸੇਸ਼ਣ</t>
+        </is>
+      </c>
+      <c r="L238" t="n">
+        <v>1</v>
+      </c>
+      <c r="M238" t="n">
+        <v>6</v>
+      </c>
+      <c r="N238" t="n">
+        <v>54730</v>
+      </c>
+      <c r="O238" t="n">
+        <v>1</v>
+      </c>
+      <c r="P238" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q238" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S238" t="inlineStr"/>
+      <c r="T238" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U238" t="inlineStr"/>
+      <c r="V238" t="inlineStr"/>
+      <c r="W238" t="inlineStr"/>
+      <c r="X238" t="inlineStr"/>
+      <c r="Y238" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z238" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA238" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB238" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC238" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਮਨੁ ਜਾਨੈ ਸਭ ਬਾਤ ਜਾਨਤ ਹੀ ਅਉਗਨੁ ਕਰੈ ॥</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr"/>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>ਅਉਗਨੁ</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>No meanings found for ਅਉਗਨੁ</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>ੁ</t>
+        </is>
+      </c>
+      <c r="G239" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>Accusative ਕਰਮ</t>
+        </is>
+      </c>
+      <c r="I239" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J239" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K239" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L239" t="n">
+        <v>1</v>
+      </c>
+      <c r="M239" t="n">
+        <v>7</v>
+      </c>
+      <c r="N239" t="n">
+        <v>54730</v>
+      </c>
+      <c r="O239" t="n">
+        <v>1</v>
+      </c>
+      <c r="P239" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q239" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S239" t="inlineStr"/>
+      <c r="T239" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U239" t="inlineStr"/>
+      <c r="V239" t="inlineStr"/>
+      <c r="W239" t="inlineStr"/>
+      <c r="X239" t="inlineStr"/>
+      <c r="Y239" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z239" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA239" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB239" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC239" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਮਨੁ ਜਾਨੈ ਸਭ ਬਾਤ ਜਾਨਤ ਹੀ ਅਉਗਨੁ ਕਰੈ ॥</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr"/>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>ਕਰੈ</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>ਕਰਦਾ ਹੈ| ਕਰਦਾ ਹੈ {ਇਕ-ਵਚਨ}</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>ਕਰੈ</t>
+        </is>
+      </c>
+      <c r="G240" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H240" t="inlineStr">
+        <is>
+          <t>Present ਵਰਤਮਾਨ</t>
+        </is>
+      </c>
+      <c r="I240" t="inlineStr">
+        <is>
+          <t>Trans / ਨਪੁਂਸਕ</t>
+        </is>
+      </c>
+      <c r="J240" t="inlineStr">
+        <is>
+          <t>3rd Person / ਅਨਯ ਪੁਰਖ</t>
+        </is>
+      </c>
+      <c r="K240" t="inlineStr">
+        <is>
+          <t>Verb / ਕਿਰਿਆ</t>
+        </is>
+      </c>
+      <c r="L240" t="n">
+        <v>1</v>
+      </c>
+      <c r="M240" t="n">
+        <v>8</v>
+      </c>
+      <c r="N240" t="n">
+        <v>54730</v>
+      </c>
+      <c r="O240" t="n">
+        <v>1</v>
+      </c>
+      <c r="P240" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q240" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S240" t="inlineStr"/>
+      <c r="T240" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U240" t="inlineStr"/>
+      <c r="V240" t="inlineStr"/>
+      <c r="W240" t="inlineStr"/>
+      <c r="X240" t="inlineStr"/>
+      <c r="Y240" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z240" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="AA240" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB240" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC240" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
New assessment of verse done
</commit_message>
<xml_diff>
--- a/1.2.1 assessment_data.xlsx
+++ b/1.2.1 assessment_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC240"/>
+  <dimension ref="A1:AC247"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25155,6 +25155,725 @@
         <v>0</v>
       </c>
     </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਕੀ ਕੁਸਲਾਤ ਹਾਥਿ ਦੀਪੁ ਕੂਏ ਪਰੈ ॥੨੧੬॥</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Why (speak) of well-being, (when) the lamp in hand falls into the well?</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr"/>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>ਕਿਸ ਵਾਸਤੇ?</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="G241" t="inlineStr"/>
+      <c r="H241" t="inlineStr">
+        <is>
+          <t>Reason / ਕਾਰਣ ਵਾਚਕ</t>
+        </is>
+      </c>
+      <c r="I241" t="inlineStr"/>
+      <c r="J241" t="inlineStr"/>
+      <c r="K241" t="inlineStr">
+        <is>
+          <t>Adverb / ਕਿਰਿਆ ਵਿਸੇਸ਼ਣ</t>
+        </is>
+      </c>
+      <c r="L241" t="n">
+        <v>1</v>
+      </c>
+      <c r="M241" t="n">
+        <v>0</v>
+      </c>
+      <c r="N241" t="n">
+        <v>54731</v>
+      </c>
+      <c r="O241" t="n">
+        <v>2</v>
+      </c>
+      <c r="P241" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q241" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S241" t="inlineStr"/>
+      <c r="T241" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U241" t="inlineStr"/>
+      <c r="V241" t="inlineStr"/>
+      <c r="W241" t="inlineStr"/>
+      <c r="X241" t="inlineStr"/>
+      <c r="Y241" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z241" t="inlineStr">
+        <is>
+          <t>Shalok End</t>
+        </is>
+      </c>
+      <c r="AA241" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB241" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC241" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਕੀ ਕੁਸਲਾਤ ਹਾਥਿ ਦੀਪੁ ਕੂਏ ਪਰੈ ॥੨੧੬॥</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Why (speak) of well-being, (when) the lamp in hand falls into the well?</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr"/>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>ਕੀ</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>ਦੀ</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>ਕੀ</t>
+        </is>
+      </c>
+      <c r="G242" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>Of</t>
+        </is>
+      </c>
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>Feminine / ਇਸਤਰੀ</t>
+        </is>
+      </c>
+      <c r="J242" t="inlineStr"/>
+      <c r="K242" t="inlineStr">
+        <is>
+          <t>Postposition / ਸੰਬੰਧਕ</t>
+        </is>
+      </c>
+      <c r="L242" t="n">
+        <v>1</v>
+      </c>
+      <c r="M242" t="n">
+        <v>1</v>
+      </c>
+      <c r="N242" t="n">
+        <v>54731</v>
+      </c>
+      <c r="O242" t="n">
+        <v>2</v>
+      </c>
+      <c r="P242" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q242" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S242" t="inlineStr"/>
+      <c r="T242" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U242" t="inlineStr"/>
+      <c r="V242" t="inlineStr"/>
+      <c r="W242" t="inlineStr"/>
+      <c r="X242" t="inlineStr"/>
+      <c r="Y242" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z242" t="inlineStr">
+        <is>
+          <t>Shalok End</t>
+        </is>
+      </c>
+      <c r="AA242" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB242" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC242" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਕੀ ਕੁਸਲਾਤ ਹਾਥਿ ਦੀਪੁ ਕੂਏ ਪਰੈ ॥੨੧੬॥</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Why (speak) of well-being, (when) the lamp in hand falls into the well?</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr"/>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>ਕੁਸਲਾਤ</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>ਸੁਖ</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ</t>
+        </is>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>Genitive ਸੰਬੰਧ</t>
+        </is>
+      </c>
+      <c r="I243" t="inlineStr">
+        <is>
+          <t>Feminine / ਇਸਤਰੀ</t>
+        </is>
+      </c>
+      <c r="J243" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K243" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L243" t="n">
+        <v>1</v>
+      </c>
+      <c r="M243" t="n">
+        <v>2</v>
+      </c>
+      <c r="N243" t="n">
+        <v>54731</v>
+      </c>
+      <c r="O243" t="n">
+        <v>2</v>
+      </c>
+      <c r="P243" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q243" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S243" t="inlineStr"/>
+      <c r="T243" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U243" t="inlineStr"/>
+      <c r="V243" t="inlineStr"/>
+      <c r="W243" t="inlineStr"/>
+      <c r="X243" t="inlineStr"/>
+      <c r="Y243" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z243" t="inlineStr">
+        <is>
+          <t>Shalok End</t>
+        </is>
+      </c>
+      <c r="AA243" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB243" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC243" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਕੀ ਕੁਸਲਾਤ ਹਾਥਿ ਦੀਪੁ ਕੂਏ ਪਰੈ ॥੨੧੬॥</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Why (speak) of well-being, (when) the lamp in hand falls into the well?</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr"/>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>ਹਾਥਿ</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>ਹੱਥ ਵਿਚ</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>ਿ</t>
+        </is>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>Locative ਅਧਿਕਰਣ</t>
+        </is>
+      </c>
+      <c r="I244" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J244" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K244" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L244" t="n">
+        <v>1</v>
+      </c>
+      <c r="M244" t="n">
+        <v>3</v>
+      </c>
+      <c r="N244" t="n">
+        <v>54731</v>
+      </c>
+      <c r="O244" t="n">
+        <v>2</v>
+      </c>
+      <c r="P244" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q244" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S244" t="inlineStr"/>
+      <c r="T244" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U244" t="inlineStr"/>
+      <c r="V244" t="inlineStr"/>
+      <c r="W244" t="inlineStr"/>
+      <c r="X244" t="inlineStr"/>
+      <c r="Y244" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z244" t="inlineStr">
+        <is>
+          <t>Shalok End</t>
+        </is>
+      </c>
+      <c r="AA244" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB244" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC244" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਕੀ ਕੁਸਲਾਤ ਹਾਥਿ ਦੀਪੁ ਕੂਏ ਪਰੈ ॥੨੧੬॥</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Why (speak) of well-being, (when) the lamp in hand falls into the well?</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr"/>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>ਦੀਪੁ</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>ਹਾਥਿ ਦੀਪੁ: ਹੱਥਾਂ ਵਿਚ ਦੀਵਾ</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>ੁ</t>
+        </is>
+      </c>
+      <c r="G245" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H245" t="inlineStr">
+        <is>
+          <t>Nominative ਕਰਤਾ</t>
+        </is>
+      </c>
+      <c r="I245" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J245" t="inlineStr">
+        <is>
+          <t>ਮੁਕਤਾ Ending</t>
+        </is>
+      </c>
+      <c r="K245" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L245" t="n">
+        <v>1</v>
+      </c>
+      <c r="M245" t="n">
+        <v>4</v>
+      </c>
+      <c r="N245" t="n">
+        <v>54731</v>
+      </c>
+      <c r="O245" t="n">
+        <v>2</v>
+      </c>
+      <c r="P245" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q245" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S245" t="inlineStr"/>
+      <c r="T245" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U245" t="inlineStr"/>
+      <c r="V245" t="inlineStr"/>
+      <c r="W245" t="inlineStr"/>
+      <c r="X245" t="inlineStr"/>
+      <c r="Y245" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z245" t="inlineStr">
+        <is>
+          <t>Shalok End</t>
+        </is>
+      </c>
+      <c r="AA245" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB245" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC245" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਕੀ ਕੁਸਲਾਤ ਹਾਥਿ ਦੀਪੁ ਕੂਏ ਪਰੈ ॥੨੧੬॥</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Why (speak) of well-being, (when) the lamp in hand falls into the well?</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr"/>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>ਕੂਏ</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>ਖੂਹ ਵਿਚ</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>ਕੂਏ</t>
+        </is>
+      </c>
+      <c r="G246" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H246" t="inlineStr">
+        <is>
+          <t>Locative ਅਧਿਕਰਣ</t>
+        </is>
+      </c>
+      <c r="I246" t="inlineStr">
+        <is>
+          <t>Masculine / ਪੁਲਿੰਗ</t>
+        </is>
+      </c>
+      <c r="J246" t="inlineStr">
+        <is>
+          <t>ਕੰਨਾ Ending</t>
+        </is>
+      </c>
+      <c r="K246" t="inlineStr">
+        <is>
+          <t>Noun / ਨਾਂਵ</t>
+        </is>
+      </c>
+      <c r="L246" t="n">
+        <v>1</v>
+      </c>
+      <c r="M246" t="n">
+        <v>5</v>
+      </c>
+      <c r="N246" t="n">
+        <v>54731</v>
+      </c>
+      <c r="O246" t="n">
+        <v>2</v>
+      </c>
+      <c r="P246" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q246" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R246" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S246" t="inlineStr"/>
+      <c r="T246" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U246" t="inlineStr"/>
+      <c r="V246" t="inlineStr"/>
+      <c r="W246" t="inlineStr"/>
+      <c r="X246" t="inlineStr"/>
+      <c r="Y246" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z246" t="inlineStr">
+        <is>
+          <t>Shalok End</t>
+        </is>
+      </c>
+      <c r="AA246" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB246" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC246" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਕੀ ਕੁਸਲਾਤ ਹਾਥਿ ਦੀਪੁ ਕੂਏ ਪਰੈ ॥੨੧੬॥</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Why (speak) of well-being, (when) the lamp in hand falls into the well?</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr"/>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>ਪਰੈ</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>ਪੜੈ| ਪੈਂਦਾ ਹੈ</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>ਕਰੈ</t>
+        </is>
+      </c>
+      <c r="G247" t="inlineStr">
+        <is>
+          <t>Singular / ਇਕ</t>
+        </is>
+      </c>
+      <c r="H247" t="inlineStr">
+        <is>
+          <t>Present ਵਰਤਮਾਨ</t>
+        </is>
+      </c>
+      <c r="I247" t="inlineStr">
+        <is>
+          <t>Trans / ਨਪੁਂਸਕ</t>
+        </is>
+      </c>
+      <c r="J247" t="inlineStr">
+        <is>
+          <t>3rd Person / ਅਨਯ ਪੁਰਖ</t>
+        </is>
+      </c>
+      <c r="K247" t="inlineStr">
+        <is>
+          <t>Verb / ਕਿਰਿਆ</t>
+        </is>
+      </c>
+      <c r="L247" t="n">
+        <v>1</v>
+      </c>
+      <c r="M247" t="n">
+        <v>6</v>
+      </c>
+      <c r="N247" t="n">
+        <v>54731</v>
+      </c>
+      <c r="O247" t="n">
+        <v>2</v>
+      </c>
+      <c r="P247" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q247" t="n">
+        <v>3818</v>
+      </c>
+      <c r="R247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ਸਲੋਕ ਭਗਤ ਕਬੀਰ ਜੀਉ ਕੇ </t>
+        </is>
+      </c>
+      <c r="S247" t="inlineStr"/>
+      <c r="T247" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਜੀ</t>
+        </is>
+      </c>
+      <c r="U247" t="inlineStr"/>
+      <c r="V247" t="inlineStr"/>
+      <c r="W247" t="inlineStr"/>
+      <c r="X247" t="inlineStr"/>
+      <c r="Y247" t="inlineStr">
+        <is>
+          <t>ਸ਼ਲੋਕ</t>
+        </is>
+      </c>
+      <c r="Z247" t="inlineStr">
+        <is>
+          <t>Shalok End</t>
+        </is>
+      </c>
+      <c r="AA247" t="n">
+        <v>1376</v>
+      </c>
+      <c r="AB247" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC247" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Prompt user for missing Translation in reanalysis flow   Description   - Problem: save_assessment_data_reanalysis raised a KeyError when new_entry lacked a Translation (and sometimes Verse) because users could skip the field during reanalysis.   - Fix: Added _ensure_translation_for_reanalysis, a guard that populates Verse from the current context when absent, prompts the user for a translation (looping until they provide text or explicitly confirm leaving it blank), and guarantees the Translation key is present before saving.   - Outcome: Reanalysis saves no longer crash, the entry schema stays consistent, and users must make a conscious choice about translations rather than skipping them silently.
  Tests
  - python -m py_compile 1.1.0_birha.py
</commit_message>
<xml_diff>
--- a/1.2.1 assessment_data.xlsx
+++ b/1.2.1 assessment_data.xlsx
@@ -24237,7 +24237,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C232" t="inlineStr"/>
+      <c r="C232" t="n">
+        <v>5</v>
+      </c>
       <c r="D232" t="inlineStr">
         <is>
           <t>ਕਬੀਰ</t>
@@ -24342,7 +24344,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C233" t="inlineStr"/>
+      <c r="C233" t="n">
+        <v>5</v>
+      </c>
       <c r="D233" t="inlineStr">
         <is>
           <t>ਮਨੁ</t>
@@ -24447,7 +24451,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C234" t="inlineStr"/>
+      <c r="C234" t="n">
+        <v>5</v>
+      </c>
       <c r="D234" t="inlineStr">
         <is>
           <t>ਜਾਨੈ</t>
@@ -24552,7 +24558,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C235" t="inlineStr"/>
+      <c r="C235" t="n">
+        <v>5</v>
+      </c>
       <c r="D235" t="inlineStr">
         <is>
           <t>ਸਭ</t>
@@ -24653,7 +24661,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C236" t="inlineStr"/>
+      <c r="C236" t="n">
+        <v>5</v>
+      </c>
       <c r="D236" t="inlineStr">
         <is>
           <t>ਬਾਤ</t>
@@ -24758,7 +24768,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C237" t="inlineStr"/>
+      <c r="C237" t="n">
+        <v>5</v>
+      </c>
       <c r="D237" t="inlineStr">
         <is>
           <t>ਜਾਨਤ</t>
@@ -24863,7 +24875,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C238" t="inlineStr"/>
+      <c r="C238" t="n">
+        <v>5</v>
+      </c>
       <c r="D238" t="inlineStr">
         <is>
           <t>ਹੀ</t>
@@ -24956,20 +24970,18 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C239" t="inlineStr"/>
+      <c r="C239" t="n">
+        <v>5</v>
+      </c>
       <c r="D239" t="inlineStr">
         <is>
           <t>ਅਉਗਨੁ</t>
         </is>
       </c>
-      <c r="E239" t="inlineStr">
-        <is>
-          <t>No meanings found for ਅਉਗਨੁ</t>
-        </is>
-      </c>
+      <c r="E239" t="inlineStr"/>
       <c r="F239" t="inlineStr">
         <is>
-          <t>ੁ</t>
+          <t>ਚੰਦਨੁ</t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
@@ -24998,7 +25010,7 @@
         </is>
       </c>
       <c r="L239" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M239" t="n">
         <v>7</v>
@@ -25061,7 +25073,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C240" t="inlineStr"/>
+      <c r="C240" t="n">
+        <v>5</v>
+      </c>
       <c r="D240" t="inlineStr">
         <is>
           <t>ਕਰੈ</t>

</xml_diff>

<commit_message>
Restrict reanalysis highlight to specific overlapping fields; exclude Vowel Ending Description:   - Limit MistyRose highlighting in the reanalysis pane to Word, Number / ਵਚਨ, Grammar / ਵਿਆਕਰਨ, Gender / ਲਿੰਗ, Word Root, and Type; ignore Vowel   Ending variants entirely.   - Normalize composite labels and assessment keys (BOM-stripping, whitespace trim) so comparisons stay consistent across single-field and composite   rules.   - Harden save_assessment_data_reanalysis to back-fill missing verse/translation values before DataFrame updates, preventing the Verse KeyError   while preserving revision tracking.
</commit_message>
<xml_diff>
--- a/1.2.1 assessment_data.xlsx
+++ b/1.2.1 assessment_data.xlsx
@@ -24237,7 +24237,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C232" t="inlineStr"/>
+      <c r="C232" t="n">
+        <v>3</v>
+      </c>
       <c r="D232" t="inlineStr">
         <is>
           <t>ਕਬੀਰ</t>
@@ -24342,7 +24344,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C233" t="inlineStr"/>
+      <c r="C233" t="n">
+        <v>3</v>
+      </c>
       <c r="D233" t="inlineStr">
         <is>
           <t>ਮਨੁ</t>
@@ -24447,7 +24451,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C234" t="inlineStr"/>
+      <c r="C234" t="n">
+        <v>3</v>
+      </c>
       <c r="D234" t="inlineStr">
         <is>
           <t>ਜਾਨੈ</t>
@@ -24552,7 +24558,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C235" t="inlineStr"/>
+      <c r="C235" t="n">
+        <v>3</v>
+      </c>
       <c r="D235" t="inlineStr">
         <is>
           <t>ਸਭ</t>
@@ -24653,7 +24661,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C236" t="inlineStr"/>
+      <c r="C236" t="n">
+        <v>3</v>
+      </c>
       <c r="D236" t="inlineStr">
         <is>
           <t>ਬਾਤ</t>
@@ -24758,7 +24768,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C237" t="inlineStr"/>
+      <c r="C237" t="n">
+        <v>3</v>
+      </c>
       <c r="D237" t="inlineStr">
         <is>
           <t>ਜਾਨਤ</t>
@@ -24863,7 +24875,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C238" t="inlineStr"/>
+      <c r="C238" t="n">
+        <v>3</v>
+      </c>
       <c r="D238" t="inlineStr">
         <is>
           <t>ਹੀ</t>
@@ -24956,7 +24970,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C239" t="inlineStr"/>
+      <c r="C239" t="n">
+        <v>3</v>
+      </c>
       <c r="D239" t="inlineStr">
         <is>
           <t>ਅਉਗਨੁ</t>
@@ -24969,7 +24985,7 @@
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>ੁ</t>
+          <t>ਚੰਦਨੁ</t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
@@ -24998,7 +25014,7 @@
         </is>
       </c>
       <c r="L239" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M239" t="n">
         <v>7</v>
@@ -25061,7 +25077,9 @@
           <t>O Kabir! The mind knows all matter; even while knowing, one indeed commits the fault.</t>
         </is>
       </c>
-      <c r="C240" t="inlineStr"/>
+      <c r="C240" t="n">
+        <v>3</v>
+      </c>
       <c r="D240" t="inlineStr">
         <is>
           <t>ਕਰੈ</t>

</xml_diff>

<commit_message>
Restrict reanalysis highlight to specific overlapping fields; exclude Vowel Ending   - Limit MistyRose comparisons to the normalized core grammar fields (Word, Number / ਵਚਨ, Grammar / ਵਿਆਕਰਨ, Gender / ਲਿੰਗ, Word Root, Type) and ignore Vowel Ending variants in both single-field and composite rules.   - Cache the normalized field tuple so every reanalysis highlight uses the same BOM-free keys without recomputing.   - Harden the reanalysis save flow by backfilling missing verse/translation values and tolerating absent columns when matching Excel rows, preventing the previous KeyErrors during saves.
</commit_message>
<xml_diff>
--- a/1.2.1 assessment_data.xlsx
+++ b/1.2.1 assessment_data.xlsx
@@ -24238,7 +24238,7 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D232" t="inlineStr">
         <is>
@@ -24345,7 +24345,7 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D233" t="inlineStr">
         <is>
@@ -24452,7 +24452,7 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D234" t="inlineStr">
         <is>
@@ -24559,7 +24559,7 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D235" t="inlineStr">
         <is>
@@ -24662,7 +24662,7 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D236" t="inlineStr">
         <is>
@@ -24769,7 +24769,7 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D237" t="inlineStr">
         <is>
@@ -24876,7 +24876,7 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D238" t="inlineStr">
         <is>
@@ -24971,7 +24971,7 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D239" t="inlineStr">
         <is>
@@ -25014,7 +25014,7 @@
         </is>
       </c>
       <c r="L239" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M239" t="n">
         <v>7</v>
@@ -25078,7 +25078,7 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D240" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Refresh reanalysis dashboard and limit reassessment prompt to current selections   1. Track and reuse only the grammar options chosen in the active reanalysis session so the ChatGPT reassessment prompt never reinserts past selections.   2. Cache the normalized highlight field tuple and reuse it across reanalysis comparisons for consistent BOM-free key handling.   3. After finishing reanalysis, refresh the “Select words to re-analyze” view (or the dashboard) on the next idle cycle so the table always reflects the latest saved data.
</commit_message>
<xml_diff>
--- a/1.2.1 assessment_data.xlsx
+++ b/1.2.1 assessment_data.xlsx
@@ -24238,7 +24238,7 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D232" t="inlineStr">
         <is>
@@ -24345,7 +24345,7 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D233" t="inlineStr">
         <is>
@@ -24452,7 +24452,7 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D234" t="inlineStr">
         <is>
@@ -24559,7 +24559,7 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D235" t="inlineStr">
         <is>
@@ -24662,7 +24662,7 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D236" t="inlineStr">
         <is>
@@ -24769,7 +24769,7 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D237" t="inlineStr">
         <is>
@@ -24876,7 +24876,7 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D238" t="inlineStr">
         <is>
@@ -24971,7 +24971,7 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D239" t="inlineStr">
         <is>
@@ -25014,7 +25014,7 @@
         </is>
       </c>
       <c r="L239" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M239" t="n">
         <v>7</v>
@@ -25078,7 +25078,7 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D240" t="inlineStr">
         <is>

</xml_diff>